<commit_message>
update bathymetry data, add DWER SW and passmore data
</commit_message>
<xml_diff>
--- a/Code/bathymetry/misc_data.xlsx
+++ b/Code/bathymetry/misc_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthipsey/Local/lake-richmond/Code/bathymetry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3B620A5-7F33-1A43-871E-E46320649FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3500436C-AB18-2545-B0D7-7C6D6AFA0A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="780" windowWidth="35900" windowHeight="27520" activeTab="3" xr2:uid="{667E3E3D-5D0F-BB43-8EE6-0D4FD2CE5FEE}"/>
+    <workbookView xWindow="10480" yWindow="500" windowWidth="35900" windowHeight="27200" activeTab="3" xr2:uid="{667E3E3D-5D0F-BB43-8EE6-0D4FD2CE5FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="NEARMAP" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="CHART" sheetId="4" r:id="rId4"/>
     <sheet name="GLM" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>HWL</t>
   </si>
@@ -52,6 +52,117 @@
   </si>
   <si>
     <t>Mar 14 2011</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>(m²)</t>
+  </si>
+  <si>
+    <t>-14.0          </t>
+  </si>
+  <si>
+    <t>-13.5          </t>
+  </si>
+  <si>
+    <t>-13.0          </t>
+  </si>
+  <si>
+    <t>-12.5          </t>
+  </si>
+  <si>
+    <t>-12.0          </t>
+  </si>
+  <si>
+    <t>-11.5          </t>
+  </si>
+  <si>
+    <t>-11.0          </t>
+  </si>
+  <si>
+    <t>-10.5          </t>
+  </si>
+  <si>
+    <t>-10.0          </t>
+  </si>
+  <si>
+    <t>-9.5           </t>
+  </si>
+  <si>
+    <t>-9.0           </t>
+  </si>
+  <si>
+    <t>-8.5           </t>
+  </si>
+  <si>
+    <t>-8.0           </t>
+  </si>
+  <si>
+    <t>-7.5           </t>
+  </si>
+  <si>
+    <t>-7.0           </t>
+  </si>
+  <si>
+    <t>-6.5           </t>
+  </si>
+  <si>
+    <t>-6.0           </t>
+  </si>
+  <si>
+    <t>-5.5           </t>
+  </si>
+  <si>
+    <t>-5.0           </t>
+  </si>
+  <si>
+    <t>-4.5           </t>
+  </si>
+  <si>
+    <t>-4.0           </t>
+  </si>
+  <si>
+    <t>-3.5           </t>
+  </si>
+  <si>
+    <t>-3.0           </t>
+  </si>
+  <si>
+    <t>-2.5           </t>
+  </si>
+  <si>
+    <t>-2.0           </t>
+  </si>
+  <si>
+    <t>-1.5           </t>
+  </si>
+  <si>
+    <t>-1.0           </t>
+  </si>
+  <si>
+    <t>-0.5           </t>
+  </si>
+  <si>
+    <t>0.0            </t>
+  </si>
+  <si>
+    <t>0.5            </t>
+  </si>
+  <si>
+    <t>1.0            </t>
+  </si>
+  <si>
+    <t>1.5            </t>
+  </si>
+  <si>
+    <t>2.0            </t>
+  </si>
+  <si>
+    <t>Contours</t>
   </si>
 </sst>
 </file>
@@ -101,11 +212,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,6 +638,257 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-EA8D-8D40-96C4-33BE1D30B02B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Brendan</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CHART!$V$3:$V$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-13.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-8.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-6.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-5.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-4.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CHART!$W$3:$W$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>13427</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19942</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27315</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77549</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>103928</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>111962</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>127971</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>135913</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>143079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150279</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>157578</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>164983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>172402</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>179995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>187685</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>195552</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>204431</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>213626</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>223178</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>233426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>248473</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>264150</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280412</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>300984</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>393251</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>519293</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>571886</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>613093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-54AF-8B44-AE47-4E17E04A8273}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -674,6 +1037,870 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.52534179542415682"/>
+          <c:y val="0.34489079082505991"/>
+          <c:w val="7.6073298915465756E-2"/>
+          <c:h val="0.14674015748031496"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10898335208098987"/>
+          <c:y val="2.5851938895417155E-2"/>
+          <c:w val="0.83478807649043874"/>
+          <c:h val="0.9482961222091657"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Contours</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CHART!$W$3:$W$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>13427</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19942</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27315</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77549</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>103928</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>111962</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>127971</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>135913</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>143079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150279</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>157578</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>164983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>172402</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>179995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>187685</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>195552</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>204431</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>213626</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>223178</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>233426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>248473</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>264150</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280412</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>300984</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>393251</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>519293</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>571886</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>613093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CHART!$V$3:$V$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-13.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-8.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-6.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-5.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-4.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A454-E142-9E13-29E8BF01DA59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Strategen</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Strategen!$F$6:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>310000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>489000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>554000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Strategen!$E$6:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A454-E142-9E13-29E8BF01DA59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Nearmap</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NEARMAP!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>410550</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>312054</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>280000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NEARMAP!$D$5:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A454-E142-9E13-29E8BF01DA59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Thesis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>THESIS!$G$3:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>575750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>246556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>THESIS!$F$3:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A454-E142-9E13-29E8BF01DA59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="409524431"/>
+        <c:axId val="409602527"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="409524431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="650000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Area (m2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.75588108868525428"/>
+              <c:y val="0.23529600140764528"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409602527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="409602527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="-15"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Depth (mAHD)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.4591949370814631E-2"/>
+              <c:y val="0.43501675977653631"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409524431"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="3"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.62524468319964677"/>
+          <c:y val="0.50155069722429946"/>
+          <c:w val="0.12148805551848392"/>
+          <c:h val="0.15083904456077071"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -787,7 +2014,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1313,10 +3096,10 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1336,6 +3119,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E5801B8-8B9F-EC44-7049-B5E64813C6AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1795,172 +3614,757 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F23296-E7B7-594A-B440-BC6312AA28EC}">
-  <dimension ref="P4:Q23"/>
+  <dimension ref="P1:BA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y54" sqref="Y54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="16:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="W2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3" s="4">
+        <v>-14</v>
+      </c>
+      <c r="W3">
+        <v>13427</v>
+      </c>
+    </row>
+    <row r="4" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P4">
         <v>2</v>
       </c>
       <c r="Q4">
         <v>900000</v>
       </c>
-    </row>
-    <row r="5" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="4">
+        <f>V3+0.5</f>
+        <v>-13.5</v>
+      </c>
+      <c r="W4">
+        <v>19942</v>
+      </c>
+    </row>
+    <row r="5" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P5" s="2">
         <v>1.07</v>
       </c>
       <c r="Q5" s="2">
         <v>570000</v>
       </c>
-    </row>
-    <row r="6" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V5" s="4">
+        <f t="shared" ref="V5:V35" si="0">V4+0.5</f>
+        <v>-13</v>
+      </c>
+      <c r="W5">
+        <v>27315</v>
+      </c>
+    </row>
+    <row r="6" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P6" s="2">
         <v>0.75</v>
       </c>
       <c r="Q6" s="2">
         <v>460000</v>
       </c>
-    </row>
-    <row r="7" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="4">
+        <f t="shared" si="0"/>
+        <v>-12.5</v>
+      </c>
+      <c r="W6">
+        <v>35557</v>
+      </c>
+    </row>
+    <row r="7" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P7" s="2">
         <v>0.26</v>
       </c>
       <c r="Q7" s="2">
         <v>290000</v>
       </c>
-    </row>
-    <row r="8" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="4">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="W7">
+        <v>54024</v>
+      </c>
+    </row>
+    <row r="8" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P8" s="2">
         <v>0</v>
       </c>
       <c r="Q8" s="3">
         <v>250000</v>
       </c>
-    </row>
-    <row r="9" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V8" s="4">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
+      <c r="W8">
+        <v>65496</v>
+      </c>
+    </row>
+    <row r="9" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P9" s="2">
         <v>-1</v>
       </c>
       <c r="Q9" s="3">
         <v>190000</v>
       </c>
-    </row>
-    <row r="10" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" s="4">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="W9">
+        <v>77549</v>
+      </c>
+    </row>
+    <row r="10" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P10" s="2">
         <v>-2</v>
       </c>
       <c r="Q10" s="3">
         <v>160000</v>
       </c>
-    </row>
-    <row r="11" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V10" s="4">
+        <f t="shared" si="0"/>
+        <v>-10.5</v>
+      </c>
+      <c r="W10">
+        <v>90308</v>
+      </c>
+    </row>
+    <row r="11" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P11" s="2">
         <v>-3</v>
       </c>
       <c r="Q11" s="3">
         <v>140000</v>
       </c>
-    </row>
-    <row r="12" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11" s="4">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="W11">
+        <v>103928</v>
+      </c>
+    </row>
+    <row r="12" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P12" s="2">
         <v>-4</v>
       </c>
       <c r="Q12" s="3">
         <v>130000</v>
       </c>
-    </row>
-    <row r="13" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V12" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.5</v>
+      </c>
+      <c r="W12">
+        <v>111962</v>
+      </c>
+    </row>
+    <row r="13" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P13" s="2">
         <v>-5</v>
       </c>
       <c r="Q13" s="3">
         <v>120000</v>
       </c>
-    </row>
-    <row r="14" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13" s="4">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="W13">
+        <v>119997</v>
+      </c>
+    </row>
+    <row r="14" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P14" s="2">
         <v>-6</v>
       </c>
       <c r="Q14" s="3">
         <v>110000</v>
       </c>
-    </row>
-    <row r="15" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.5</v>
+      </c>
+      <c r="W14">
+        <v>127971</v>
+      </c>
+    </row>
+    <row r="15" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P15" s="2">
         <v>-7</v>
       </c>
       <c r="Q15" s="3">
         <v>100000</v>
       </c>
-    </row>
-    <row r="16" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V15" s="4">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="W15">
+        <v>135913</v>
+      </c>
+    </row>
+    <row r="16" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P16" s="2">
         <v>-8</v>
       </c>
       <c r="Q16" s="3">
         <v>90000</v>
       </c>
-    </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.5</v>
+      </c>
+      <c r="W16">
+        <v>143079</v>
+      </c>
+    </row>
+    <row r="17" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P17" s="2">
         <v>-9</v>
       </c>
       <c r="Q17" s="3">
         <v>80000</v>
       </c>
-    </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="W17">
+        <v>150279</v>
+      </c>
+    </row>
+    <row r="18" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P18" s="2">
         <v>-10</v>
       </c>
       <c r="Q18" s="3">
         <v>70000</v>
       </c>
-    </row>
-    <row r="19" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V18" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.5</v>
+      </c>
+      <c r="W18">
+        <v>157578</v>
+      </c>
+    </row>
+    <row r="19" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P19" s="2">
         <v>-11</v>
       </c>
       <c r="Q19" s="3">
         <v>60000</v>
       </c>
-    </row>
-    <row r="20" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V19" s="4">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="W19">
+        <v>164983</v>
+      </c>
+    </row>
+    <row r="20" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P20" s="2">
         <v>-12</v>
       </c>
       <c r="Q20" s="3">
         <v>45000</v>
       </c>
-    </row>
-    <row r="21" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V20" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.5</v>
+      </c>
+      <c r="W20">
+        <v>172402</v>
+      </c>
+    </row>
+    <row r="21" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P21" s="2">
         <v>-13</v>
       </c>
       <c r="Q21" s="3">
         <v>20000</v>
       </c>
-    </row>
-    <row r="22" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="W21">
+        <v>179995</v>
+      </c>
+    </row>
+    <row r="22" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P22" s="2">
         <v>-14</v>
       </c>
       <c r="Q22" s="3">
         <v>8000</v>
       </c>
-    </row>
-    <row r="23" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="U22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V22" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.5</v>
+      </c>
+      <c r="W22">
+        <v>187685</v>
+      </c>
+    </row>
+    <row r="23" spans="16:23" x14ac:dyDescent="0.2">
       <c r="P23" s="2">
         <v>-14.6</v>
       </c>
       <c r="Q23" s="2">
         <v>0.1</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V23" s="4">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="W23">
+        <v>195552</v>
+      </c>
+    </row>
+    <row r="24" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V24" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.5</v>
+      </c>
+      <c r="W24">
+        <v>204431</v>
+      </c>
+    </row>
+    <row r="25" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="W25">
+        <v>213626</v>
+      </c>
+    </row>
+    <row r="26" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V26" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.5</v>
+      </c>
+      <c r="W26">
+        <v>223178</v>
+      </c>
+    </row>
+    <row r="27" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="V27" s="4">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="W27">
+        <v>233426</v>
+      </c>
+    </row>
+    <row r="28" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V28" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
+      <c r="W28">
+        <v>248473</v>
+      </c>
+    </row>
+    <row r="29" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V29" s="4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="W29">
+        <v>264150</v>
+      </c>
+    </row>
+    <row r="30" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V30" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="W30">
+        <v>280412</v>
+      </c>
+    </row>
+    <row r="31" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>300984</v>
+      </c>
+    </row>
+    <row r="32" spans="16:23" x14ac:dyDescent="0.2">
+      <c r="U32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="W32">
+        <v>393251</v>
+      </c>
+    </row>
+    <row r="33" spans="19:53" x14ac:dyDescent="0.2">
+      <c r="U33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V33" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>519293</v>
+      </c>
+    </row>
+    <row r="34" spans="19:53" x14ac:dyDescent="0.2">
+      <c r="U34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V34" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W34">
+        <v>571886</v>
+      </c>
+    </row>
+    <row r="35" spans="19:53" x14ac:dyDescent="0.2">
+      <c r="U35" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V35" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W35">
+        <v>613093</v>
+      </c>
+    </row>
+    <row r="39" spans="19:53" x14ac:dyDescent="0.2">
+      <c r="S39">
+        <v>-14.5</v>
+      </c>
+      <c r="T39">
+        <v>-14</v>
+      </c>
+      <c r="U39">
+        <v>-13.5</v>
+      </c>
+      <c r="V39">
+        <v>-13</v>
+      </c>
+      <c r="W39">
+        <v>-12.5</v>
+      </c>
+      <c r="X39">
+        <v>-12</v>
+      </c>
+      <c r="Y39">
+        <v>-11.5</v>
+      </c>
+      <c r="Z39">
+        <v>-11</v>
+      </c>
+      <c r="AA39">
+        <v>-10.5</v>
+      </c>
+      <c r="AB39">
+        <v>-10</v>
+      </c>
+      <c r="AC39">
+        <v>-9.5</v>
+      </c>
+      <c r="AD39">
+        <v>-9</v>
+      </c>
+      <c r="AE39">
+        <v>-8.5</v>
+      </c>
+      <c r="AF39">
+        <v>-8</v>
+      </c>
+      <c r="AG39">
+        <v>-7.5</v>
+      </c>
+      <c r="AH39">
+        <v>-7</v>
+      </c>
+      <c r="AI39">
+        <v>-6.5</v>
+      </c>
+      <c r="AJ39">
+        <v>-6</v>
+      </c>
+      <c r="AK39">
+        <v>-5.5</v>
+      </c>
+      <c r="AL39">
+        <v>-5</v>
+      </c>
+      <c r="AM39">
+        <v>-4.5</v>
+      </c>
+      <c r="AN39">
+        <v>-4</v>
+      </c>
+      <c r="AO39">
+        <v>-3.5</v>
+      </c>
+      <c r="AP39">
+        <v>-3</v>
+      </c>
+      <c r="AQ39">
+        <v>-2.5</v>
+      </c>
+      <c r="AR39">
+        <v>-2</v>
+      </c>
+      <c r="AS39">
+        <v>-1.5</v>
+      </c>
+      <c r="AT39">
+        <v>-1</v>
+      </c>
+      <c r="AU39">
+        <v>-0.5</v>
+      </c>
+      <c r="AV39">
+        <v>0</v>
+      </c>
+      <c r="AW39">
+        <v>0.5</v>
+      </c>
+      <c r="AX39">
+        <v>1</v>
+      </c>
+      <c r="AY39">
+        <v>1.5</v>
+      </c>
+      <c r="AZ39">
+        <v>2</v>
+      </c>
+      <c r="BA39">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="40" spans="19:53" x14ac:dyDescent="0.2">
+      <c r="S40">
+        <v>2000</v>
+      </c>
+      <c r="T40">
+        <v>13427</v>
+      </c>
+      <c r="U40">
+        <v>19942</v>
+      </c>
+      <c r="V40">
+        <v>27315</v>
+      </c>
+      <c r="W40">
+        <v>35557</v>
+      </c>
+      <c r="X40">
+        <v>54024</v>
+      </c>
+      <c r="Y40">
+        <v>65496</v>
+      </c>
+      <c r="Z40">
+        <v>77549</v>
+      </c>
+      <c r="AA40">
+        <v>90308</v>
+      </c>
+      <c r="AB40">
+        <v>103928</v>
+      </c>
+      <c r="AC40">
+        <v>111962</v>
+      </c>
+      <c r="AD40">
+        <v>119997</v>
+      </c>
+      <c r="AE40">
+        <v>127971</v>
+      </c>
+      <c r="AF40">
+        <v>135913</v>
+      </c>
+      <c r="AG40">
+        <v>143079</v>
+      </c>
+      <c r="AH40">
+        <v>150279</v>
+      </c>
+      <c r="AI40">
+        <v>157578</v>
+      </c>
+      <c r="AJ40">
+        <v>164983</v>
+      </c>
+      <c r="AK40">
+        <v>172402</v>
+      </c>
+      <c r="AL40">
+        <v>179995</v>
+      </c>
+      <c r="AM40">
+        <v>187685</v>
+      </c>
+      <c r="AN40">
+        <v>195552</v>
+      </c>
+      <c r="AO40">
+        <v>204431</v>
+      </c>
+      <c r="AP40">
+        <v>213626</v>
+      </c>
+      <c r="AQ40">
+        <v>223178</v>
+      </c>
+      <c r="AR40">
+        <v>233426</v>
+      </c>
+      <c r="AS40">
+        <v>248473</v>
+      </c>
+      <c r="AT40">
+        <v>264150</v>
+      </c>
+      <c r="AU40">
+        <v>280412</v>
+      </c>
+      <c r="AV40">
+        <v>300984</v>
+      </c>
+      <c r="AW40">
+        <v>393251</v>
+      </c>
+      <c r="AX40">
+        <v>519293</v>
+      </c>
+      <c r="AY40">
+        <v>571886</v>
+      </c>
+      <c r="AZ40">
+        <v>613093</v>
+      </c>
+      <c r="BA40">
+        <v>650000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to water balance and glm
</commit_message>
<xml_diff>
--- a/Code/bathymetry/misc_data.xlsx
+++ b/Code/bathymetry/misc_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthipsey/Local/lake-richmond/Code/bathymetry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3500436C-AB18-2545-B0D7-7C6D6AFA0A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06D5772-DC94-C446-AE6B-E1C5E1C2A214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10480" yWindow="500" windowWidth="35900" windowHeight="27200" activeTab="3" xr2:uid="{667E3E3D-5D0F-BB43-8EE6-0D4FD2CE5FEE}"/>
   </bookViews>
@@ -3616,8 +3616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F23296-E7B7-594A-B440-BC6312AA28EC}">
   <dimension ref="P1:BA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y54" sqref="Y54"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AY43" sqref="AY43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4151,6 +4151,113 @@
       </c>
       <c r="W35">
         <v>613093</v>
+      </c>
+    </row>
+    <row r="38" spans="19:53" x14ac:dyDescent="0.2">
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>2</v>
+      </c>
+      <c r="U38">
+        <v>3</v>
+      </c>
+      <c r="V38">
+        <v>4</v>
+      </c>
+      <c r="W38">
+        <v>5</v>
+      </c>
+      <c r="X38">
+        <v>6</v>
+      </c>
+      <c r="Y38">
+        <v>7</v>
+      </c>
+      <c r="Z38">
+        <v>8</v>
+      </c>
+      <c r="AA38">
+        <v>9</v>
+      </c>
+      <c r="AB38">
+        <v>10</v>
+      </c>
+      <c r="AC38">
+        <v>11</v>
+      </c>
+      <c r="AD38">
+        <v>12</v>
+      </c>
+      <c r="AE38">
+        <v>13</v>
+      </c>
+      <c r="AF38">
+        <v>14</v>
+      </c>
+      <c r="AG38">
+        <v>15</v>
+      </c>
+      <c r="AH38">
+        <v>16</v>
+      </c>
+      <c r="AI38">
+        <v>17</v>
+      </c>
+      <c r="AJ38">
+        <v>18</v>
+      </c>
+      <c r="AK38">
+        <v>19</v>
+      </c>
+      <c r="AL38">
+        <v>20</v>
+      </c>
+      <c r="AM38">
+        <v>21</v>
+      </c>
+      <c r="AN38">
+        <v>22</v>
+      </c>
+      <c r="AO38">
+        <v>23</v>
+      </c>
+      <c r="AP38">
+        <v>24</v>
+      </c>
+      <c r="AQ38">
+        <v>25</v>
+      </c>
+      <c r="AR38">
+        <v>26</v>
+      </c>
+      <c r="AS38">
+        <v>27</v>
+      </c>
+      <c r="AT38">
+        <v>28</v>
+      </c>
+      <c r="AU38">
+        <v>29</v>
+      </c>
+      <c r="AV38">
+        <v>30</v>
+      </c>
+      <c r="AW38">
+        <v>31</v>
+      </c>
+      <c r="AX38">
+        <v>32</v>
+      </c>
+      <c r="AY38">
+        <v>33</v>
+      </c>
+      <c r="AZ38">
+        <v>34</v>
+      </c>
+      <c r="BA38">
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="19:53" x14ac:dyDescent="0.2">

</xml_diff>